<commit_message>
round 2 formatting and database merge
</commit_message>
<xml_diff>
--- a/data/lit_review/round1/raw/20250618_depuration_biotoxin_marine_ocean_sea_plus.xlsx
+++ b/data/lit_review/round1/raw/20250618_depuration_biotoxin_marine_ocean_sea_plus.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10921"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11003"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/UCSB/projects/hab_depuration/data/lit_review/round1/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{535D652F-9CF8-3943-AA12-B19A0DBC3EA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAC563B2-8F66-1D44-AE9B-8C33AD10D04F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1320" yWindow="500" windowWidth="33120" windowHeight="20180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11291" uniqueCount="1317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11291" uniqueCount="1316">
   <si>
     <t>Article Title</t>
   </si>
@@ -3900,9 +3900,6 @@
   </si>
   <si>
     <t>Table 5???</t>
-  </si>
-  <si>
-    <t>reported</t>
   </si>
   <si>
     <t>Year 1</t>
@@ -4183,7 +4180,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4216,7 +4213,6 @@
     <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4534,8 +4530,8 @@
   <dimension ref="A1:Z555"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A220" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C228" sqref="C228"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
@@ -7815,16 +7811,16 @@
         <v>430</v>
       </c>
       <c r="P49" s="24" t="s">
+        <v>538</v>
+      </c>
+      <c r="Q49" s="24" t="s">
         <v>629</v>
       </c>
-      <c r="Q49" s="24" t="s">
-        <v>538</v>
-      </c>
       <c r="R49" s="24" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="S49" s="24" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="T49" s="24" t="s">
         <v>870</v>
@@ -7880,16 +7876,16 @@
         <v>430</v>
       </c>
       <c r="P50" s="24" t="s">
+        <v>538</v>
+      </c>
+      <c r="Q50" s="24" t="s">
         <v>629</v>
       </c>
-      <c r="Q50" s="24" t="s">
-        <v>538</v>
-      </c>
       <c r="R50" s="24" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="S50" s="24" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="T50" s="24" t="s">
         <v>870</v>
@@ -7945,16 +7941,16 @@
         <v>722</v>
       </c>
       <c r="P51" s="24" t="s">
+        <v>538</v>
+      </c>
+      <c r="Q51" s="24" t="s">
         <v>629</v>
       </c>
-      <c r="Q51" s="24" t="s">
-        <v>538</v>
-      </c>
       <c r="R51" s="24" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="S51" s="24" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="T51" s="24" t="s">
         <v>870</v>
@@ -8010,16 +8006,16 @@
         <v>722</v>
       </c>
       <c r="P52" s="24" t="s">
+        <v>538</v>
+      </c>
+      <c r="Q52" s="24" t="s">
         <v>629</v>
       </c>
-      <c r="Q52" s="24" t="s">
-        <v>538</v>
-      </c>
       <c r="R52" s="24" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="S52" s="24" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="T52" s="24" t="s">
         <v>870</v>
@@ -8075,16 +8071,16 @@
         <v>722</v>
       </c>
       <c r="P53" s="24" t="s">
+        <v>595</v>
+      </c>
+      <c r="Q53" s="24" t="s">
         <v>629</v>
       </c>
-      <c r="Q53" s="24" t="s">
-        <v>595</v>
-      </c>
       <c r="R53" s="24" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="S53" s="24" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
       <c r="T53" s="24" t="s">
         <v>870</v>
@@ -8141,16 +8137,16 @@
         <v>722</v>
       </c>
       <c r="P54" s="24" t="s">
+        <v>595</v>
+      </c>
+      <c r="Q54" s="24" t="s">
         <v>629</v>
       </c>
-      <c r="Q54" s="24" t="s">
-        <v>595</v>
-      </c>
       <c r="R54" s="24" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="S54" s="24" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="T54" s="24" t="s">
         <v>870</v>
@@ -8207,16 +8203,16 @@
         <v>722</v>
       </c>
       <c r="P55" s="24" t="s">
+        <v>595</v>
+      </c>
+      <c r="Q55" s="24" t="s">
         <v>629</v>
       </c>
-      <c r="Q55" s="24" t="s">
-        <v>595</v>
-      </c>
       <c r="R55" s="24" t="s">
+        <v>1289</v>
+      </c>
+      <c r="S55" s="24" t="s">
         <v>1290</v>
-      </c>
-      <c r="S55" s="24" t="s">
-        <v>1291</v>
       </c>
       <c r="T55" s="24" t="s">
         <v>870</v>
@@ -8273,16 +8269,16 @@
         <v>722</v>
       </c>
       <c r="P56" s="24" t="s">
+        <v>595</v>
+      </c>
+      <c r="Q56" s="24" t="s">
         <v>629</v>
       </c>
-      <c r="Q56" s="24" t="s">
-        <v>595</v>
-      </c>
       <c r="R56" s="24" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="S56" s="24" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="T56" s="24" t="s">
         <v>870</v>
@@ -8339,16 +8335,16 @@
         <v>430</v>
       </c>
       <c r="P57" s="24" t="s">
+        <v>538</v>
+      </c>
+      <c r="Q57" s="24" t="s">
         <v>629</v>
       </c>
-      <c r="Q57" s="24" t="s">
-        <v>538</v>
-      </c>
       <c r="R57" s="24" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="S57" s="24" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="T57" s="24" t="s">
         <v>870</v>
@@ -8405,16 +8401,16 @@
         <v>430</v>
       </c>
       <c r="P58" s="24" t="s">
+        <v>538</v>
+      </c>
+      <c r="Q58" s="24" t="s">
         <v>629</v>
       </c>
-      <c r="Q58" s="24" t="s">
-        <v>538</v>
-      </c>
       <c r="R58" s="24" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="S58" s="24" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="T58" s="24" t="s">
         <v>870</v>
@@ -8471,16 +8467,16 @@
         <v>430</v>
       </c>
       <c r="P59" s="24" t="s">
+        <v>538</v>
+      </c>
+      <c r="Q59" s="24" t="s">
         <v>629</v>
       </c>
-      <c r="Q59" s="24" t="s">
-        <v>538</v>
-      </c>
       <c r="R59" s="24" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="S59" s="24" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="T59" s="24" t="s">
         <v>870</v>
@@ -8537,16 +8533,16 @@
         <v>430</v>
       </c>
       <c r="P60" s="24" t="s">
+        <v>538</v>
+      </c>
+      <c r="Q60" s="24" t="s">
         <v>629</v>
       </c>
-      <c r="Q60" s="24" t="s">
-        <v>538</v>
-      </c>
       <c r="R60" s="24" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="S60" s="24" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="T60" s="24" t="s">
         <v>870</v>
@@ -10822,7 +10818,7 @@
         <v>483</v>
       </c>
       <c r="M95" s="24" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="N95" s="24" t="s">
         <v>452</v>
@@ -10834,7 +10830,7 @@
         <v>566</v>
       </c>
       <c r="Q95" s="24" t="s">
-        <v>1278</v>
+        <v>617</v>
       </c>
       <c r="R95" s="24" t="s">
         <v>998</v>
@@ -10849,7 +10845,7 @@
         <v>-4.9416349999999998E-3</v>
       </c>
       <c r="Y95" s="24" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="96" spans="1:25">
@@ -10890,7 +10886,7 @@
         <v>483</v>
       </c>
       <c r="M96" s="24" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="N96" s="24" t="s">
         <v>452</v>
@@ -10902,7 +10898,7 @@
         <v>566</v>
       </c>
       <c r="Q96" s="24" t="s">
-        <v>1278</v>
+        <v>617</v>
       </c>
       <c r="R96" s="24" t="s">
         <v>998</v>
@@ -10917,7 +10913,7 @@
         <v>-3.1779439999999998E-3</v>
       </c>
       <c r="Y96" s="24" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="97" spans="1:25">
@@ -18599,10 +18595,10 @@
         <v>633</v>
       </c>
       <c r="R216" s="24" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
       <c r="S216" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="T216" s="24" t="s">
         <v>870</v>
@@ -18666,10 +18662,10 @@
         <v>633</v>
       </c>
       <c r="R217" s="24" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
       <c r="S217" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
       <c r="T217" s="24" t="s">
         <v>870</v>
@@ -18696,7 +18692,7 @@
       <c r="E218" s="24" t="s">
         <v>208</v>
       </c>
-      <c r="F218" s="30" t="s">
+      <c r="F218" s="24" t="s">
         <v>206</v>
       </c>
       <c r="G218" s="24" t="s">
@@ -18733,10 +18729,10 @@
         <v>633</v>
       </c>
       <c r="R218" s="24" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
       <c r="S218" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="T218" s="24" t="s">
         <v>870</v>
@@ -18763,7 +18759,7 @@
       <c r="E219" s="24" t="s">
         <v>208</v>
       </c>
-      <c r="F219" s="30" t="s">
+      <c r="F219" s="24" t="s">
         <v>206</v>
       </c>
       <c r="G219" s="24" t="s">
@@ -18800,10 +18796,10 @@
         <v>633</v>
       </c>
       <c r="R219" s="24" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
       <c r="S219" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
       <c r="T219" s="24" t="s">
         <v>870</v>
@@ -19633,381 +19629,381 @@
         <v>875</v>
       </c>
     </row>
-    <row r="232" spans="1:25" s="30" customFormat="1">
-      <c r="A232" s="30" t="s">
+    <row r="232" spans="1:25">
+      <c r="A232" s="24" t="s">
         <v>993</v>
       </c>
-      <c r="B232" s="30">
+      <c r="B232" s="24">
         <v>98</v>
       </c>
-      <c r="C232" s="30" t="s">
+      <c r="C232" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="D232" s="30" t="s">
-        <v>392</v>
-      </c>
-      <c r="E232" s="30" t="s">
+      <c r="D232" s="24" t="s">
+        <v>392</v>
+      </c>
+      <c r="E232" s="24" t="s">
         <v>208</v>
       </c>
-      <c r="F232" s="30" t="s">
+      <c r="F232" s="24" t="s">
         <v>206</v>
       </c>
-      <c r="G232" s="30" t="s">
+      <c r="G232" s="24" t="s">
         <v>358</v>
       </c>
-      <c r="H232" s="30" t="s">
+      <c r="H232" s="24" t="s">
         <v>312</v>
       </c>
-      <c r="I232" s="30" t="s">
+      <c r="I232" s="24" t="s">
         <v>311</v>
       </c>
-      <c r="J232" s="30" t="s">
+      <c r="J232" s="24" t="s">
         <v>1051</v>
       </c>
-      <c r="K232" s="30" t="s">
+      <c r="K232" s="24" t="s">
         <v>394</v>
       </c>
-      <c r="L232" s="30" t="s">
-        <v>405</v>
-      </c>
-      <c r="M232" s="30" t="s">
-        <v>405</v>
-      </c>
-      <c r="N232" s="30" t="s">
+      <c r="L232" s="24" t="s">
+        <v>405</v>
+      </c>
+      <c r="M232" s="24" t="s">
+        <v>405</v>
+      </c>
+      <c r="N232" s="24" t="s">
         <v>398</v>
       </c>
-      <c r="O232" s="30" t="s">
+      <c r="O232" s="24" t="s">
         <v>457</v>
       </c>
-      <c r="P232" s="30" t="s">
+      <c r="P232" s="24" t="s">
         <v>579</v>
       </c>
-      <c r="Q232" s="30" t="s">
+      <c r="Q232" s="24" t="s">
         <v>633</v>
       </c>
-      <c r="R232" s="30" t="s">
+      <c r="R232" s="24" t="s">
         <v>1027</v>
       </c>
-      <c r="S232" s="30" t="s">
+      <c r="S232" s="24" t="s">
         <v>1097</v>
       </c>
-      <c r="T232" s="30" t="s">
+      <c r="T232" s="24" t="s">
         <v>870</v>
       </c>
     </row>
-    <row r="233" spans="1:25" s="30" customFormat="1">
-      <c r="A233" s="30" t="s">
+    <row r="233" spans="1:25">
+      <c r="A233" s="24" t="s">
         <v>993</v>
       </c>
-      <c r="B233" s="30">
+      <c r="B233" s="24">
         <v>98</v>
       </c>
-      <c r="C233" s="30" t="s">
+      <c r="C233" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="D233" s="30" t="s">
-        <v>392</v>
-      </c>
-      <c r="E233" s="30" t="s">
+      <c r="D233" s="24" t="s">
+        <v>392</v>
+      </c>
+      <c r="E233" s="24" t="s">
         <v>208</v>
       </c>
-      <c r="F233" s="30" t="s">
+      <c r="F233" s="24" t="s">
         <v>206</v>
       </c>
-      <c r="G233" s="30" t="s">
+      <c r="G233" s="24" t="s">
         <v>358</v>
       </c>
-      <c r="H233" s="30" t="s">
+      <c r="H233" s="24" t="s">
         <v>312</v>
       </c>
-      <c r="I233" s="30" t="s">
+      <c r="I233" s="24" t="s">
         <v>311</v>
       </c>
-      <c r="J233" s="30" t="s">
+      <c r="J233" s="24" t="s">
         <v>1051</v>
       </c>
-      <c r="K233" s="30" t="s">
+      <c r="K233" s="24" t="s">
         <v>394</v>
       </c>
-      <c r="L233" s="30" t="s">
-        <v>405</v>
-      </c>
-      <c r="M233" s="30" t="s">
-        <v>405</v>
-      </c>
-      <c r="N233" s="30" t="s">
+      <c r="L233" s="24" t="s">
+        <v>405</v>
+      </c>
+      <c r="M233" s="24" t="s">
+        <v>405</v>
+      </c>
+      <c r="N233" s="24" t="s">
         <v>398</v>
       </c>
-      <c r="O233" s="30" t="s">
+      <c r="O233" s="24" t="s">
         <v>400</v>
       </c>
-      <c r="P233" s="30" t="s">
+      <c r="P233" s="24" t="s">
         <v>579</v>
       </c>
-      <c r="Q233" s="30" t="s">
+      <c r="Q233" s="24" t="s">
         <v>633</v>
       </c>
-      <c r="R233" s="30" t="s">
+      <c r="R233" s="24" t="s">
         <v>1027</v>
       </c>
-      <c r="S233" s="30" t="s">
+      <c r="S233" s="24" t="s">
         <v>1096</v>
       </c>
-      <c r="T233" s="30" t="s">
+      <c r="T233" s="24" t="s">
         <v>870</v>
       </c>
     </row>
-    <row r="234" spans="1:25" s="30" customFormat="1">
-      <c r="A234" s="30" t="s">
+    <row r="234" spans="1:25">
+      <c r="A234" s="24" t="s">
         <v>993</v>
       </c>
-      <c r="B234" s="30">
+      <c r="B234" s="24">
         <v>98</v>
       </c>
-      <c r="C234" s="30" t="s">
+      <c r="C234" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="D234" s="30" t="s">
-        <v>392</v>
-      </c>
-      <c r="E234" s="30" t="s">
+      <c r="D234" s="24" t="s">
+        <v>392</v>
+      </c>
+      <c r="E234" s="24" t="s">
         <v>208</v>
       </c>
-      <c r="F234" s="30" t="s">
+      <c r="F234" s="24" t="s">
         <v>206</v>
       </c>
-      <c r="G234" s="30" t="s">
+      <c r="G234" s="24" t="s">
         <v>358</v>
       </c>
-      <c r="H234" s="30" t="s">
+      <c r="H234" s="24" t="s">
         <v>312</v>
       </c>
-      <c r="I234" s="30" t="s">
-        <v>1311</v>
-      </c>
-      <c r="J234" s="30" t="s">
+      <c r="I234" s="24" t="s">
+        <v>1310</v>
+      </c>
+      <c r="J234" s="24" t="s">
         <v>1051</v>
       </c>
-      <c r="K234" s="30" t="s">
+      <c r="K234" s="24" t="s">
         <v>394</v>
       </c>
-      <c r="L234" s="30" t="s">
-        <v>405</v>
-      </c>
-      <c r="M234" s="30" t="s">
-        <v>405</v>
-      </c>
-      <c r="N234" s="30" t="s">
+      <c r="L234" s="24" t="s">
+        <v>405</v>
+      </c>
+      <c r="M234" s="24" t="s">
+        <v>405</v>
+      </c>
+      <c r="N234" s="24" t="s">
         <v>398</v>
       </c>
-      <c r="O234" s="30" t="s">
+      <c r="O234" s="24" t="s">
         <v>457</v>
       </c>
-      <c r="P234" s="30" t="s">
+      <c r="P234" s="24" t="s">
         <v>579</v>
       </c>
-      <c r="Q234" s="30" t="s">
+      <c r="Q234" s="24" t="s">
         <v>633</v>
       </c>
-      <c r="R234" s="30" t="s">
+      <c r="R234" s="24" t="s">
         <v>1027</v>
       </c>
-      <c r="S234" s="30" t="s">
+      <c r="S234" s="24" t="s">
         <v>1274</v>
       </c>
-      <c r="T234" s="30" t="s">
+      <c r="T234" s="24" t="s">
         <v>870</v>
       </c>
     </row>
-    <row r="235" spans="1:25" s="30" customFormat="1">
-      <c r="A235" s="30" t="s">
+    <row r="235" spans="1:25">
+      <c r="A235" s="24" t="s">
         <v>993</v>
       </c>
-      <c r="B235" s="30">
+      <c r="B235" s="24">
         <v>98</v>
       </c>
-      <c r="C235" s="30" t="s">
+      <c r="C235" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="D235" s="30" t="s">
-        <v>392</v>
-      </c>
-      <c r="E235" s="30" t="s">
+      <c r="D235" s="24" t="s">
+        <v>392</v>
+      </c>
+      <c r="E235" s="24" t="s">
         <v>208</v>
       </c>
-      <c r="F235" s="30" t="s">
+      <c r="F235" s="24" t="s">
         <v>206</v>
       </c>
-      <c r="G235" s="30" t="s">
+      <c r="G235" s="24" t="s">
         <v>358</v>
       </c>
-      <c r="H235" s="30" t="s">
+      <c r="H235" s="24" t="s">
         <v>312</v>
       </c>
-      <c r="I235" s="30" t="s">
-        <v>1311</v>
-      </c>
-      <c r="J235" s="30" t="s">
+      <c r="I235" s="24" t="s">
+        <v>1310</v>
+      </c>
+      <c r="J235" s="24" t="s">
         <v>1051</v>
       </c>
-      <c r="K235" s="30" t="s">
+      <c r="K235" s="24" t="s">
         <v>394</v>
       </c>
-      <c r="L235" s="30" t="s">
-        <v>405</v>
-      </c>
-      <c r="M235" s="30" t="s">
-        <v>405</v>
-      </c>
-      <c r="N235" s="30" t="s">
+      <c r="L235" s="24" t="s">
+        <v>405</v>
+      </c>
+      <c r="M235" s="24" t="s">
+        <v>405</v>
+      </c>
+      <c r="N235" s="24" t="s">
         <v>398</v>
       </c>
-      <c r="O235" s="30" t="s">
+      <c r="O235" s="24" t="s">
         <v>400</v>
       </c>
-      <c r="P235" s="30" t="s">
+      <c r="P235" s="24" t="s">
         <v>579</v>
       </c>
-      <c r="Q235" s="30" t="s">
+      <c r="Q235" s="24" t="s">
         <v>633</v>
       </c>
-      <c r="R235" s="30" t="s">
+      <c r="R235" s="24" t="s">
         <v>1027</v>
       </c>
-      <c r="S235" s="30" t="s">
+      <c r="S235" s="24" t="s">
         <v>1273</v>
       </c>
-      <c r="T235" s="30" t="s">
+      <c r="T235" s="24" t="s">
         <v>870</v>
       </c>
     </row>
-    <row r="236" spans="1:25" s="30" customFormat="1">
-      <c r="A236" s="30" t="s">
+    <row r="236" spans="1:25">
+      <c r="A236" s="24" t="s">
         <v>901</v>
       </c>
-      <c r="B236" s="30">
+      <c r="B236" s="24">
         <v>33</v>
       </c>
-      <c r="C236" s="30" t="s">
+      <c r="C236" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="D236" s="30" t="s">
-        <v>392</v>
-      </c>
-      <c r="E236" s="30" t="s">
+      <c r="D236" s="24" t="s">
+        <v>392</v>
+      </c>
+      <c r="E236" s="24" t="s">
         <v>542</v>
       </c>
-      <c r="F236" s="30" t="s">
+      <c r="F236" s="24" t="s">
         <v>313</v>
       </c>
-      <c r="G236" s="30" t="s">
+      <c r="G236" s="24" t="s">
         <v>358</v>
       </c>
-      <c r="H236" s="30" t="s">
+      <c r="H236" s="24" t="s">
         <v>312</v>
       </c>
-      <c r="I236" s="30" t="s">
+      <c r="I236" s="24" t="s">
         <v>358</v>
       </c>
-      <c r="J236" s="30" t="s">
+      <c r="J236" s="24" t="s">
         <v>543</v>
       </c>
-      <c r="K236" s="30" t="s">
+      <c r="K236" s="24" t="s">
         <v>394</v>
       </c>
-      <c r="L236" s="30" t="s">
-        <v>405</v>
-      </c>
-      <c r="M236" s="30" t="s">
-        <v>405</v>
-      </c>
-      <c r="N236" s="30" t="s">
+      <c r="L236" s="24" t="s">
+        <v>405</v>
+      </c>
+      <c r="M236" s="24" t="s">
+        <v>405</v>
+      </c>
+      <c r="N236" s="24" t="s">
         <v>398</v>
       </c>
-      <c r="O236" s="30" t="s">
+      <c r="O236" s="24" t="s">
         <v>408</v>
       </c>
-      <c r="P236" s="30" t="s">
+      <c r="P236" s="24" t="s">
         <v>536</v>
       </c>
-      <c r="Q236" s="30" t="s">
+      <c r="Q236" s="24" t="s">
         <v>617</v>
       </c>
-      <c r="R236" s="30" t="s">
-        <v>998</v>
-      </c>
-      <c r="S236" s="30" t="s">
-        <v>998</v>
-      </c>
-      <c r="T236" s="30" t="s">
+      <c r="R236" s="24" t="s">
+        <v>998</v>
+      </c>
+      <c r="S236" s="24" t="s">
+        <v>998</v>
+      </c>
+      <c r="T236" s="24" t="s">
         <v>872</v>
       </c>
-      <c r="U236" s="30">
+      <c r="U236" s="24">
         <v>-0.93054999999999999</v>
       </c>
     </row>
-    <row r="237" spans="1:25" s="30" customFormat="1">
-      <c r="A237" s="30" t="s">
+    <row r="237" spans="1:25">
+      <c r="A237" s="24" t="s">
         <v>901</v>
       </c>
-      <c r="B237" s="30">
+      <c r="B237" s="24">
         <v>33</v>
       </c>
-      <c r="C237" s="30" t="s">
+      <c r="C237" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="D237" s="30" t="s">
-        <v>392</v>
-      </c>
-      <c r="E237" s="30" t="s">
+      <c r="D237" s="24" t="s">
+        <v>392</v>
+      </c>
+      <c r="E237" s="24" t="s">
         <v>542</v>
       </c>
-      <c r="F237" s="30" t="s">
+      <c r="F237" s="24" t="s">
         <v>313</v>
       </c>
-      <c r="G237" s="30" t="s">
+      <c r="G237" s="24" t="s">
         <v>358</v>
       </c>
-      <c r="H237" s="30" t="s">
+      <c r="H237" s="24" t="s">
         <v>312</v>
       </c>
-      <c r="I237" s="30" t="s">
+      <c r="I237" s="24" t="s">
         <v>358</v>
       </c>
-      <c r="J237" s="30" t="s">
+      <c r="J237" s="24" t="s">
         <v>311</v>
       </c>
-      <c r="K237" s="30" t="s">
+      <c r="K237" s="24" t="s">
         <v>394</v>
       </c>
-      <c r="L237" s="30" t="s">
-        <v>405</v>
-      </c>
-      <c r="M237" s="30" t="s">
-        <v>405</v>
-      </c>
-      <c r="N237" s="30" t="s">
+      <c r="L237" s="24" t="s">
+        <v>405</v>
+      </c>
+      <c r="M237" s="24" t="s">
+        <v>405</v>
+      </c>
+      <c r="N237" s="24" t="s">
         <v>398</v>
       </c>
-      <c r="O237" s="30" t="s">
+      <c r="O237" s="24" t="s">
         <v>408</v>
       </c>
-      <c r="P237" s="30" t="s">
+      <c r="P237" s="24" t="s">
         <v>536</v>
       </c>
-      <c r="Q237" s="30" t="s">
+      <c r="Q237" s="24" t="s">
         <v>617</v>
       </c>
-      <c r="R237" s="30" t="s">
-        <v>998</v>
-      </c>
-      <c r="S237" s="30" t="s">
-        <v>998</v>
-      </c>
-      <c r="T237" s="30" t="s">
+      <c r="R237" s="24" t="s">
+        <v>998</v>
+      </c>
+      <c r="S237" s="24" t="s">
+        <v>998</v>
+      </c>
+      <c r="T237" s="24" t="s">
         <v>872</v>
       </c>
-      <c r="U237" s="30">
+      <c r="U237" s="24">
         <v>-4.9863999999999999E-2</v>
       </c>
     </row>
@@ -22491,7 +22487,7 @@
         <v>291</v>
       </c>
       <c r="I276" s="23" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="J276" s="23" t="s">
         <v>707</v>
@@ -22560,7 +22556,7 @@
         <v>291</v>
       </c>
       <c r="I277" s="23" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="J277" s="23" t="s">
         <v>597</v>
@@ -22629,7 +22625,7 @@
         <v>291</v>
       </c>
       <c r="I278" s="23" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="J278" s="23" t="s">
         <v>623</v>
@@ -22698,7 +22694,7 @@
         <v>291</v>
       </c>
       <c r="I279" s="23" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="J279" s="23" t="s">
         <v>1051</v>
@@ -24940,7 +24936,7 @@
         <v>343</v>
       </c>
       <c r="I312" s="24" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
       <c r="J312" s="24" t="s">
         <v>1051</v>
@@ -25005,7 +25001,7 @@
         <v>343</v>
       </c>
       <c r="I313" s="24" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
       <c r="J313" s="24" t="s">
         <v>1051</v>
@@ -25070,7 +25066,7 @@
         <v>343</v>
       </c>
       <c r="I314" s="24" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
       <c r="J314" s="24" t="s">
         <v>1051</v>
@@ -25135,7 +25131,7 @@
         <v>343</v>
       </c>
       <c r="I315" s="24" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
       <c r="J315" s="24" t="s">
         <v>1051</v>
@@ -25780,7 +25776,7 @@
         <v>-0.152941176470588</v>
       </c>
       <c r="X324" s="24">
-        <f>LN(2)/ABS(W324)</f>
+        <f t="shared" ref="X324:X341" si="0">LN(2)/ABS(W324)</f>
         <v>4.5321161805842651</v>
       </c>
       <c r="Y324" s="23" t="s">
@@ -25854,7 +25850,7 @@
         <v>-0.25581395348837199</v>
       </c>
       <c r="X325" s="24">
-        <f>LN(2)/ABS(W325)</f>
+        <f t="shared" si="0"/>
         <v>2.7095753421888782</v>
       </c>
       <c r="Y325" s="23" t="s">
@@ -25928,7 +25924,7 @@
         <v>-0.435294117647058</v>
       </c>
       <c r="X326" s="24">
-        <f>LN(2)/ABS(W326)</f>
+        <f t="shared" si="0"/>
         <v>1.592365144529607</v>
       </c>
       <c r="Y326" s="23" t="s">
@@ -26002,7 +25998,7 @@
         <v>-0.435294117647058</v>
       </c>
       <c r="X327" s="24">
-        <f>LN(2)/ABS(W327)</f>
+        <f t="shared" si="0"/>
         <v>1.592365144529607</v>
       </c>
       <c r="Y327" s="23" t="s">
@@ -26076,7 +26072,7 @@
         <v>-0.45882352941176402</v>
       </c>
       <c r="X328" s="24">
-        <f>LN(2)/ABS(W328)</f>
+        <f t="shared" si="0"/>
         <v>1.5107053935280881</v>
       </c>
       <c r="Y328" s="23" t="s">
@@ -26150,7 +26146,7 @@
         <v>-0.46511627906976699</v>
       </c>
       <c r="X329" s="24">
-        <f>LN(2)/ABS(W329)</f>
+        <f t="shared" si="0"/>
         <v>1.4902664382038837</v>
       </c>
       <c r="Y329" s="23" t="s">
@@ -26224,7 +26220,7 @@
         <v>-0.623529411764706</v>
       </c>
       <c r="X330" s="24">
-        <f>LN(2)/ABS(W330)</f>
+        <f t="shared" si="0"/>
         <v>1.1116511386338743</v>
       </c>
       <c r="Y330" s="23" t="s">
@@ -26298,7 +26294,7 @@
         <v>-0.89534883720930203</v>
       </c>
       <c r="X331" s="24">
-        <f>LN(2)/ABS(W331)</f>
+        <f t="shared" si="0"/>
         <v>0.77416438348253658</v>
       </c>
       <c r="Y331" s="23" t="s">
@@ -26372,7 +26368,7 @@
         <v>-0.94117647058823495</v>
       </c>
       <c r="X332" s="24">
-        <f>LN(2)/ABS(W332)</f>
+        <f t="shared" si="0"/>
         <v>0.7364688793449421</v>
       </c>
       <c r="Y332" s="23" t="s">
@@ -26446,7 +26442,7 @@
         <v>-1</v>
       </c>
       <c r="X333" s="24">
-        <f>LN(2)/ABS(W333)</f>
+        <f t="shared" si="0"/>
         <v>0.69314718055994529</v>
       </c>
       <c r="Y333" s="23" t="s">
@@ -26520,7 +26516,7 @@
         <v>-1.3411764705882301</v>
       </c>
       <c r="X334" s="24">
-        <f>LN(2)/ABS(W334)</f>
+        <f t="shared" si="0"/>
         <v>0.51682026620697874</v>
       </c>
       <c r="Y334" s="23" t="s">
@@ -26594,7 +26590,7 @@
         <v>-1.3764705882352899</v>
       </c>
       <c r="X335" s="24">
-        <f>LN(2)/ABS(W335)</f>
+        <f t="shared" si="0"/>
         <v>0.50356846450936354</v>
       </c>
       <c r="Y335" s="23" t="s">
@@ -26668,7 +26664,7 @@
         <v>-1.3953488372092999</v>
       </c>
       <c r="X336" s="24">
-        <f>LN(2)/ABS(W336)</f>
+        <f t="shared" si="0"/>
         <v>0.496755479401295</v>
       </c>
       <c r="Y336" s="23" t="s">
@@ -26742,7 +26738,7 @@
         <v>-1.48235294117647</v>
       </c>
       <c r="X337" s="24">
-        <f>LN(2)/ABS(W337)</f>
+        <f t="shared" si="0"/>
         <v>0.46759928847297916</v>
       </c>
       <c r="Y337" s="23" t="s">
@@ -26816,7 +26812,7 @@
         <v>-1.5930232558139501</v>
       </c>
       <c r="X338" s="24">
-        <f>LN(2)/ABS(W338)</f>
+        <f t="shared" si="0"/>
         <v>0.43511428852668188</v>
       </c>
       <c r="Y338" s="23" t="s">
@@ -26890,7 +26886,7 @@
         <v>-1.6162790697674401</v>
       </c>
       <c r="X339" s="24">
-        <f>LN(2)/ABS(W339)</f>
+        <f t="shared" si="0"/>
         <v>0.42885365128169323</v>
       </c>
       <c r="Y339" s="23" t="s">
@@ -26964,7 +26960,7 @@
         <v>-1.74117647058823</v>
       </c>
       <c r="X340" s="24">
-        <f>LN(2)/ABS(W340)</f>
+        <f t="shared" si="0"/>
         <v>0.39809128613240224</v>
       </c>
       <c r="Y340" s="23" t="s">
@@ -27038,7 +27034,7 @@
         <v>-2.0588235294117601</v>
       </c>
       <c r="X341" s="24">
-        <f>LN(2)/ABS(W341)</f>
+        <f t="shared" si="0"/>
         <v>0.33667148770054561</v>
       </c>
       <c r="Y341" s="23" t="s">
@@ -27822,7 +27818,7 @@
         <v>291</v>
       </c>
       <c r="I353" s="23" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="J353" s="23" t="s">
         <v>598</v>
@@ -27889,7 +27885,7 @@
         <v>291</v>
       </c>
       <c r="I354" s="23" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="J354" s="23" t="s">
         <v>597</v>
@@ -27956,7 +27952,7 @@
         <v>291</v>
       </c>
       <c r="I355" s="23" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="J355" s="24" t="s">
         <v>1051</v>
@@ -28303,7 +28299,7 @@
         <v>318</v>
       </c>
       <c r="I361" s="23" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="J361" s="23" t="s">
         <v>598</v>
@@ -28370,7 +28366,7 @@
         <v>318</v>
       </c>
       <c r="I362" s="23" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="J362" s="23" t="s">
         <v>597</v>
@@ -28437,7 +28433,7 @@
         <v>318</v>
       </c>
       <c r="I363" s="23" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="J363" s="23" t="s">
         <v>596</v>
@@ -28504,7 +28500,7 @@
         <v>318</v>
       </c>
       <c r="I364" s="23" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="J364" s="23" t="s">
         <v>1051</v>
@@ -30997,7 +30993,7 @@
         <v>318</v>
       </c>
       <c r="I402" s="23" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="J402" s="24" t="s">
         <v>597</v>
@@ -31065,7 +31061,7 @@
         <v>318</v>
       </c>
       <c r="I403" s="23" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="J403" s="24" t="s">
         <v>602</v>
@@ -31133,7 +31129,7 @@
         <v>316</v>
       </c>
       <c r="I404" s="23" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="J404" s="24" t="s">
         <v>627</v>
@@ -31204,7 +31200,7 @@
         <v>316</v>
       </c>
       <c r="I405" s="23" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="J405" s="24" t="s">
         <v>597</v>
@@ -31275,7 +31271,7 @@
         <v>316</v>
       </c>
       <c r="I406" s="23" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="J406" s="24" t="s">
         <v>574</v>
@@ -32288,7 +32284,7 @@
         <v>460</v>
       </c>
       <c r="Y421" s="24" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="422" spans="1:25">
@@ -33308,10 +33304,10 @@
         <v>291</v>
       </c>
       <c r="I437" s="23" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="J437" s="23" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="K437" s="23" t="s">
         <v>394</v>
@@ -33371,10 +33367,10 @@
         <v>291</v>
       </c>
       <c r="I438" s="23" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="J438" s="23" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="K438" s="23" t="s">
         <v>394</v>
@@ -33434,10 +33430,10 @@
         <v>291</v>
       </c>
       <c r="I439" s="23" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="J439" s="23" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
       <c r="K439" s="23" t="s">
         <v>394</v>
@@ -33497,10 +33493,10 @@
         <v>291</v>
       </c>
       <c r="I440" s="23" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="J440" s="23" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="K440" s="23" t="s">
         <v>394</v>
@@ -33560,10 +33556,10 @@
         <v>291</v>
       </c>
       <c r="I441" s="23" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="J441" s="23" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="K441" s="23" t="s">
         <v>394</v>
@@ -33623,10 +33619,10 @@
         <v>291</v>
       </c>
       <c r="I442" s="23" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="J442" s="23" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="K442" s="23" t="s">
         <v>394</v>
@@ -33813,7 +33809,7 @@
         <v>283</v>
       </c>
       <c r="J445" s="24" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="K445" s="24" t="s">
         <v>394</v>
@@ -33875,7 +33871,7 @@
         <v>283</v>
       </c>
       <c r="J446" s="24" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="K446" s="24" t="s">
         <v>394</v>
@@ -33937,7 +33933,7 @@
         <v>283</v>
       </c>
       <c r="J447" s="24" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
       <c r="K447" s="24" t="s">
         <v>394</v>
@@ -33999,7 +33995,7 @@
         <v>283</v>
       </c>
       <c r="J448" s="24" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
       <c r="K448" s="24" t="s">
         <v>394</v>
@@ -34061,7 +34057,7 @@
         <v>283</v>
       </c>
       <c r="J449" s="24" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
       <c r="K449" s="24" t="s">
         <v>394</v>
@@ -34123,7 +34119,7 @@
         <v>283</v>
       </c>
       <c r="J450" s="24" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
       <c r="K450" s="24" t="s">
         <v>394</v>
@@ -34185,7 +34181,7 @@
         <v>283</v>
       </c>
       <c r="J451" s="24" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="K451" s="24" t="s">
         <v>394</v>
@@ -34247,7 +34243,7 @@
         <v>283</v>
       </c>
       <c r="J452" s="24" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="K452" s="24" t="s">
         <v>394</v>
@@ -34309,7 +34305,7 @@
         <v>283</v>
       </c>
       <c r="J453" s="24" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
       <c r="K453" s="24" t="s">
         <v>394</v>
@@ -34371,7 +34367,7 @@
         <v>283</v>
       </c>
       <c r="J454" s="24" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
       <c r="K454" s="24" t="s">
         <v>394</v>
@@ -34433,7 +34429,7 @@
         <v>283</v>
       </c>
       <c r="J455" s="24" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="K455" s="24" t="s">
         <v>394</v>
@@ -34495,7 +34491,7 @@
         <v>283</v>
       </c>
       <c r="J456" s="24" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="K456" s="24" t="s">
         <v>394</v>
@@ -35108,7 +35104,7 @@
         <v>-2.9499999999999998E-2</v>
       </c>
       <c r="Y466" s="24" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="467" spans="1:25">
@@ -35176,7 +35172,7 @@
         <v>-7.5600000000000001E-2</v>
       </c>
       <c r="Y467" s="24" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="468" spans="1:25">
@@ -37290,7 +37286,7 @@
         <v>417</v>
       </c>
       <c r="I500" s="24" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="J500" s="24" t="s">
         <v>598</v>
@@ -37355,7 +37351,7 @@
         <v>417</v>
       </c>
       <c r="I501" s="24" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="J501" s="24" t="s">
         <v>610</v>
@@ -37420,7 +37416,7 @@
         <v>417</v>
       </c>
       <c r="I502" s="24" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="J502" s="24" t="s">
         <v>597</v>
@@ -37485,7 +37481,7 @@
         <v>417</v>
       </c>
       <c r="I503" s="24" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="J503" s="24" t="s">
         <v>611</v>
@@ -37550,7 +37546,7 @@
         <v>417</v>
       </c>
       <c r="I504" s="24" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="J504" s="24" t="s">
         <v>596</v>
@@ -37615,7 +37611,7 @@
         <v>647</v>
       </c>
       <c r="I505" s="24" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="J505" s="24" t="s">
         <v>598</v>
@@ -37680,7 +37676,7 @@
         <v>647</v>
       </c>
       <c r="I506" s="24" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="J506" s="24" t="s">
         <v>598</v>
@@ -37745,7 +37741,7 @@
         <v>647</v>
       </c>
       <c r="I507" s="24" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="J507" s="24" t="s">
         <v>610</v>
@@ -37810,7 +37806,7 @@
         <v>647</v>
       </c>
       <c r="I508" s="24" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="J508" s="24" t="s">
         <v>610</v>
@@ -37875,7 +37871,7 @@
         <v>647</v>
       </c>
       <c r="I509" s="24" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="J509" s="24" t="s">
         <v>597</v>
@@ -37940,7 +37936,7 @@
         <v>647</v>
       </c>
       <c r="I510" s="24" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="J510" s="24" t="s">
         <v>597</v>
@@ -38005,7 +38001,7 @@
         <v>647</v>
       </c>
       <c r="I511" s="24" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="J511" s="24" t="s">
         <v>611</v>
@@ -38070,7 +38066,7 @@
         <v>647</v>
       </c>
       <c r="I512" s="24" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="J512" s="24" t="s">
         <v>611</v>

</xml_diff>